<commit_message>
new compm2 stuff + renames
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C576A942-9024-4050-BE7C-8866608083D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69123B92-5B52-4D1B-A5BD-1F7B008D4D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="311">
   <si>
     <t>new</t>
   </si>
@@ -566,24 +566,9 @@
     <t>SIG Sauer BRAVO4 4X30</t>
   </si>
   <si>
-    <t>qrp_30mm_mount</t>
-  </si>
-  <si>
-    <t>QRP 30mm</t>
-  </si>
-  <si>
-    <t>aimpoint_30mm_low_ring</t>
-  </si>
-  <si>
     <t>Aimpoint 30mm Low Ring</t>
   </si>
   <si>
-    <t>comp_m2</t>
-  </si>
-  <si>
-    <t>CompM2</t>
-  </si>
-  <si>
     <t>zenit_belomo_picatinny_mount_pkas</t>
   </si>
   <si>
@@ -954,6 +939,33 @@
   </si>
   <si>
     <t>Aimpoint Micro NVG High Rise</t>
+  </si>
+  <si>
+    <t>aimpoint_30mm_low_ring_mount</t>
+  </si>
+  <si>
+    <t>aimpoint_qrp1_30mm_mount</t>
+  </si>
+  <si>
+    <t>Aimpoint QRP 30mm</t>
+  </si>
+  <si>
+    <t>aimpoint_qrp1_30mm_mount_w_spacer</t>
+  </si>
+  <si>
+    <t>Aimpoint QRP 30mm w 39mm Spacer</t>
+  </si>
+  <si>
+    <t>wilcox_compm_30mm_mount</t>
+  </si>
+  <si>
+    <t>Wilcox COMP-M 30mm</t>
+  </si>
+  <si>
+    <t>aimpoint_compm2_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint CompM2</t>
   </si>
 </sst>
 </file>
@@ -1795,20 +1807,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S178"/>
+  <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="21" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="21" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1826,7 +1838,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1879,7 +1891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1912,7 +1924,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1978,7 +1990,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2017,7 +2029,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2056,7 +2068,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2095,7 +2107,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2134,12 +2146,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C10" s="1">
         <v>-2</v>
@@ -2170,7 +2182,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2193,7 +2205,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -2259,7 +2271,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2292,7 +2304,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2317,7 +2329,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2353,12 +2365,12 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C17" s="1">
         <v>-1.5</v>
@@ -2389,7 +2401,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2412,7 +2424,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2437,7 +2449,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2462,7 +2474,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2487,7 +2499,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N22" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2497,12 +2509,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C23">
         <v>-2</v>
@@ -2522,7 +2534,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2547,7 +2559,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -2572,7 +2584,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -2597,7 +2609,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2647,7 +2659,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2672,7 +2684,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2697,7 +2709,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2725,7 +2737,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2750,7 +2762,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2775,7 +2787,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2825,7 +2837,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2850,7 +2862,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2878,7 +2890,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2906,7 +2918,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2962,12 +2974,12 @@
         <v>896</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2983,7 +2995,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -3042,7 +3054,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -3067,7 +3079,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>107</v>
       </c>
@@ -3092,7 +3104,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3117,7 +3129,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3142,7 +3154,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N48" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3152,7 +3164,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -3177,7 +3189,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -3202,7 +3214,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>115</v>
       </c>
@@ -3227,7 +3239,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -3258,7 +3270,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N53" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3268,12 +3280,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
       <c r="B54" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C54">
         <v>-2</v>
@@ -3299,12 +3311,12 @@
         <v>659</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>120</v>
       </c>
       <c r="B55" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C55">
         <v>-2</v>
@@ -3330,12 +3342,12 @@
         <v>601</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -3358,12 +3370,12 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C57">
         <v>-2</v>
@@ -3389,12 +3401,12 @@
         <v>649</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3414,12 +3426,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -3439,12 +3451,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C60">
         <v>-1</v>
@@ -3464,12 +3476,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>130</v>
       </c>
       <c r="B61" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3489,12 +3501,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -3514,12 +3526,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C63">
         <v>-2</v>
@@ -3542,12 +3554,12 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -3567,12 +3579,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C65">
         <v>-1</v>
@@ -3592,12 +3604,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3617,12 +3629,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3642,12 +3654,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>133</v>
       </c>
       <c r="B68" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3667,12 +3679,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
       <c r="B69" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3692,9 +3704,9 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N70" s="1">
-        <f t="shared" ref="N70:N99" si="7">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
+        <f t="shared" ref="N70:N101" si="7">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
         <v>0</v>
       </c>
       <c r="Q70">
@@ -3702,7 +3714,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3719,15 +3731,15 @@
         <v>200</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" ref="N71:N81" si="8">C71-D71*20-E71*0.8-F71*0.6-H71*5+I71*10+J71/300</f>
+        <f t="shared" ref="N71:N83" si="8">C71-D71*20-E71*0.8-F71*0.6-H71*5+I71*10+J71/300</f>
         <v>-0.8</v>
       </c>
       <c r="Q71">
-        <f t="shared" ref="Q71:Q81" si="9">P71*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q71:Q83" si="9">P71*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>161</v>
       </c>
@@ -3755,7 +3767,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -3780,7 +3792,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N74" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3790,12 +3802,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>179</v>
+        <v>302</v>
       </c>
       <c r="B75" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C75">
         <v>-0.5</v>
@@ -3815,50 +3827,50 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>177</v>
+        <v>303</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>304</v>
       </c>
       <c r="C76">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D76">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M76">
         <v>300</v>
       </c>
       <c r="N76" s="1">
         <f t="shared" si="8"/>
-        <v>-2.2000000000000002</v>
+        <v>-1.9000000000000001</v>
       </c>
       <c r="Q76">
         <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>181</v>
+        <v>305</v>
       </c>
       <c r="B77" t="s">
-        <v>182</v>
+        <v>306</v>
       </c>
       <c r="C77">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="D77">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="M77">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="N77" s="1">
         <f t="shared" si="8"/>
-        <v>-4.2</v>
+        <v>-2.8</v>
       </c>
       <c r="P77">
         <v>7.1</v>
@@ -3868,315 +3880,301 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" t="s">
+        <v>308</v>
+      </c>
+      <c r="C78">
+        <v>-1</v>
+      </c>
+      <c r="D78">
+        <v>0.06</v>
+      </c>
+      <c r="M78">
+        <v>600</v>
+      </c>
       <c r="N78" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Q78">
-        <f t="shared" si="9"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>309</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>310</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D79">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="M79">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="N79" s="1">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="Q79">
-        <f t="shared" si="9"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>185</v>
-      </c>
-      <c r="B80" t="s">
-        <v>186</v>
-      </c>
-      <c r="C80">
-        <v>-2</v>
-      </c>
-      <c r="D80">
-        <v>0.17</v>
-      </c>
-      <c r="M80">
-        <v>1000</v>
-      </c>
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N80" s="1">
         <f t="shared" si="8"/>
-        <v>-5.4</v>
-      </c>
-      <c r="P80">
-        <v>15.8</v>
+        <v>0</v>
       </c>
       <c r="Q80">
         <f t="shared" si="9"/>
-        <v>0.22539999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0.05</v>
+      </c>
+      <c r="M81">
+        <v>300</v>
+      </c>
       <c r="N81" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q81">
         <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>180</v>
+      </c>
+      <c r="B82" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82">
+        <v>-2</v>
+      </c>
+      <c r="D82">
+        <v>0.17</v>
+      </c>
+      <c r="M82">
+        <v>1000</v>
+      </c>
+      <c r="N82" s="1">
+        <f t="shared" si="8"/>
+        <v>-5.4</v>
+      </c>
+      <c r="P82">
+        <v>15.8</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="9"/>
+        <v>0.22539999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N83" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="9"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>135</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>136</v>
       </c>
-      <c r="C82">
+      <c r="C84">
         <v>-2.5</v>
       </c>
-      <c r="D82">
+      <c r="D84">
         <v>0.06</v>
       </c>
-      <c r="M82">
+      <c r="M84">
         <v>900</v>
       </c>
-      <c r="N82" s="1">
+      <c r="N84" s="1">
         <f t="shared" si="7"/>
         <v>-3.7</v>
       </c>
-      <c r="P82">
+      <c r="P84">
         <v>3.1746569999999998</v>
       </c>
-      <c r="Q82">
-        <f t="shared" ref="Q82:Q105" si="10">P82*0.013+0.02</f>
+      <c r="Q84">
+        <f t="shared" ref="Q84:Q107" si="10">P84*0.013+0.02</f>
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>137</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>138</v>
       </c>
-      <c r="C83">
+      <c r="C85">
         <v>-2</v>
       </c>
-      <c r="D83">
+      <c r="D85">
         <v>0.12</v>
       </c>
-      <c r="M83">
+      <c r="M85">
         <v>1000</v>
       </c>
-      <c r="N83" s="1">
+      <c r="N85" s="1">
         <f t="shared" si="7"/>
         <v>-4.4000000000000004</v>
       </c>
-      <c r="P83">
+      <c r="P85">
         <v>8</v>
       </c>
-      <c r="Q83">
+      <c r="Q85">
         <f t="shared" si="10"/>
         <v>0.124</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>139</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>140</v>
       </c>
-      <c r="C84">
+      <c r="C86">
         <v>-2.5</v>
       </c>
-      <c r="D84">
+      <c r="D86">
         <v>0.09</v>
       </c>
-      <c r="M84">
+      <c r="M86">
         <v>1000</v>
       </c>
-      <c r="N84" s="1">
+      <c r="N86" s="1">
         <f t="shared" si="7"/>
         <v>-4.3</v>
       </c>
-      <c r="P84">
+      <c r="P86">
         <v>5.6085599999999998</v>
       </c>
-      <c r="Q84">
+      <c r="Q86">
         <f t="shared" si="10"/>
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>143</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>144</v>
       </c>
-      <c r="C85">
+      <c r="C87">
         <v>-2</v>
       </c>
-      <c r="D85">
+      <c r="D87">
         <v>0.19</v>
       </c>
-      <c r="M85">
+      <c r="M87">
         <v>800</v>
       </c>
-      <c r="N85" s="1">
+      <c r="N87" s="1">
         <f t="shared" si="7"/>
         <v>-5.8</v>
       </c>
-      <c r="P85">
+      <c r="P87">
         <v>13.4041</v>
       </c>
-      <c r="Q85">
+      <c r="Q87">
         <f t="shared" si="10"/>
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>145</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>146</v>
       </c>
-      <c r="C86">
+      <c r="C88">
         <v>-6</v>
       </c>
-      <c r="D86">
+      <c r="D88">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H86">
+      <c r="H88">
         <v>0.25</v>
       </c>
-      <c r="M86">
+      <c r="M88">
         <v>600</v>
       </c>
-      <c r="N86" s="1">
+      <c r="N88" s="1">
         <f t="shared" si="7"/>
         <v>-8.65</v>
       </c>
-      <c r="P86">
+      <c r="P88">
         <v>4</v>
       </c>
-      <c r="Q86">
+      <c r="Q88">
         <f t="shared" si="10"/>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>147</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>148</v>
       </c>
-      <c r="C87">
+      <c r="C89">
         <v>-7</v>
       </c>
-      <c r="D87">
+      <c r="D89">
         <v>0.19</v>
       </c>
-      <c r="H87">
+      <c r="H89">
         <v>0.25</v>
       </c>
-      <c r="M87">
+      <c r="M89">
         <v>2000</v>
       </c>
-      <c r="N87" s="1">
+      <c r="N89" s="1">
         <f t="shared" si="7"/>
         <v>-12.05</v>
       </c>
-      <c r="P87">
+      <c r="P89">
         <v>9.6</v>
       </c>
-      <c r="Q87">
+      <c r="Q89">
         <f t="shared" si="10"/>
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>157</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>158</v>
-      </c>
-      <c r="C88">
-        <v>-2</v>
-      </c>
-      <c r="D88">
-        <v>0.16</v>
-      </c>
-      <c r="M88">
-        <v>1000</v>
-      </c>
-      <c r="N88" s="1">
-        <f t="shared" si="7"/>
-        <v>-5.2</v>
-      </c>
-      <c r="P88">
-        <v>10.5116</v>
-      </c>
-      <c r="Q88">
-        <f t="shared" si="10"/>
-        <v>0.15665079999999998</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" t="s">
-        <v>142</v>
-      </c>
-      <c r="C89">
-        <v>-2</v>
-      </c>
-      <c r="D89">
-        <v>0.16</v>
-      </c>
-      <c r="M89">
-        <v>1200</v>
-      </c>
-      <c r="N89" s="1">
-        <f t="shared" si="7"/>
-        <v>-5.2</v>
-      </c>
-      <c r="P89">
-        <v>10.93493</v>
-      </c>
-      <c r="Q89">
-        <f t="shared" si="10"/>
-        <v>0.16215408999999997</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>149</v>
-      </c>
-      <c r="B90" t="s">
-        <v>150</v>
       </c>
       <c r="C90">
         <v>-2</v>
@@ -4192,301 +4190,304 @@
         <v>-5.2</v>
       </c>
       <c r="P90">
-        <v>10.9</v>
+        <v>10.5116</v>
       </c>
       <c r="Q90">
         <f t="shared" si="10"/>
-        <v>0.16169999999999998</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.15665079999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B91" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C91">
-        <v>-2.5</v>
+        <v>-2</v>
       </c>
       <c r="D91">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="M91">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="N91" s="1">
         <f t="shared" si="7"/>
-        <v>-6.5</v>
+        <v>-5.2</v>
       </c>
       <c r="P91">
-        <v>13.9</v>
+        <v>10.93493</v>
       </c>
       <c r="Q91">
         <f t="shared" si="10"/>
-        <v>0.20069999999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.16215408999999997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B92" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C92">
         <v>-2</v>
       </c>
       <c r="D92">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="M92">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N92" s="1">
         <f t="shared" si="7"/>
-        <v>-5.4</v>
+        <v>-5.2</v>
+      </c>
+      <c r="P92">
+        <v>10.9</v>
       </c>
       <c r="Q92">
         <f t="shared" si="10"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.16169999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B93" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C93">
-        <v>-4</v>
+        <v>-2.5</v>
       </c>
       <c r="D93">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="M93">
-        <v>1600</v>
+        <v>800</v>
       </c>
       <c r="N93" s="1">
         <f t="shared" si="7"/>
-        <v>-7.4</v>
+        <v>-6.5</v>
       </c>
       <c r="P93">
-        <v>11.6</v>
+        <v>13.9</v>
       </c>
       <c r="Q93">
         <f t="shared" si="10"/>
-        <v>0.17079999999999998</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.20069999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94">
+        <v>-2</v>
+      </c>
+      <c r="D94">
+        <v>0.17</v>
+      </c>
+      <c r="M94">
+        <v>500</v>
+      </c>
       <c r="N94" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-5.4</v>
       </c>
       <c r="Q94">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C95" s="1">
-        <v>0</v>
-      </c>
-      <c r="D95" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
-      <c r="M95" s="1">
-        <v>400</v>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>155</v>
+      </c>
+      <c r="B95" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95">
+        <v>-4</v>
+      </c>
+      <c r="D95">
+        <v>0.17</v>
+      </c>
+      <c r="M95">
+        <v>1600</v>
       </c>
       <c r="N95" s="1">
         <f t="shared" si="7"/>
-        <v>-0.8</v>
+        <v>-7.4</v>
+      </c>
+      <c r="P95">
+        <v>11.6</v>
       </c>
       <c r="Q95">
         <f t="shared" si="10"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C96" s="1">
-        <v>0</v>
-      </c>
-      <c r="D96" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
-      <c r="M96" s="1">
-        <v>200</v>
-      </c>
+        <v>0.17079999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N96" s="1">
         <f t="shared" si="7"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="Q96">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>53</v>
-      </c>
-      <c r="B97" t="s">
-        <v>54</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="D97">
-        <v>0.03</v>
-      </c>
-      <c r="M97">
-        <v>350</v>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1">
+        <v>400</v>
       </c>
       <c r="N97" s="1">
         <f t="shared" si="7"/>
-        <v>-0.6</v>
+        <v>-0.8</v>
       </c>
       <c r="Q97">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>55</v>
-      </c>
-      <c r="B98" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98">
-        <v>0.03</v>
-      </c>
-      <c r="M98">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1">
         <v>200</v>
       </c>
       <c r="N98" s="1">
         <f t="shared" si="7"/>
-        <v>-0.6</v>
+        <v>-0.4</v>
       </c>
       <c r="Q98">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="M99">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="N99" s="1">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>-0.6</v>
       </c>
       <c r="Q99">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B100" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C100">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="M100">
-        <v>1200</v>
+        <v>200</v>
       </c>
       <c r="N100" s="1">
-        <f t="shared" ref="N100:N105" si="11">C100-D100*20-E100*0.8-F100*0.6-H100*5+I100*10+J100/300</f>
-        <v>-5</v>
-      </c>
-      <c r="P100">
-        <v>6.1</v>
+        <f t="shared" si="7"/>
+        <v>-0.6</v>
       </c>
       <c r="Q100">
         <f t="shared" si="10"/>
-        <v>9.9299999999999999E-2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B101" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C101">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="M101">
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="N101" s="1">
-        <f t="shared" si="11"/>
-        <v>-5</v>
+        <f t="shared" si="7"/>
+        <v>-1</v>
       </c>
       <c r="Q101">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B102" t="s">
         <v>58</v>
@@ -4498,20 +4499,23 @@
         <v>0.1</v>
       </c>
       <c r="M102">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N102" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N102:N107" si="11">C102-D102*20-E102*0.8-F102*0.6-H102*5+I102*10+J102/300</f>
         <v>-5</v>
+      </c>
+      <c r="P102">
+        <v>6.1</v>
       </c>
       <c r="Q102">
         <f t="shared" si="10"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B103" t="s">
         <v>58</v>
@@ -4523,7 +4527,7 @@
         <v>0.1</v>
       </c>
       <c r="M103">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N103" s="1">
         <f t="shared" si="11"/>
@@ -4534,579 +4538,570 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B104" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C104">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="D104">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="M104">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="N104" s="1">
         <f t="shared" si="11"/>
-        <v>-2.6</v>
-      </c>
-      <c r="P104">
-        <v>5.5</v>
+        <v>-5</v>
       </c>
       <c r="Q104">
         <f t="shared" si="10"/>
-        <v>9.1499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" t="s">
+        <v>58</v>
+      </c>
+      <c r="C105">
+        <v>-3</v>
+      </c>
+      <c r="D105">
+        <v>0.1</v>
+      </c>
+      <c r="M105">
+        <v>1500</v>
+      </c>
       <c r="N105" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="Q105">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="B106" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D106">
+        <v>0.08</v>
+      </c>
+      <c r="M106">
+        <v>1300</v>
+      </c>
+      <c r="N106" s="1">
+        <f t="shared" si="11"/>
+        <v>-2.6</v>
+      </c>
+      <c r="P106">
+        <v>5.5</v>
+      </c>
+      <c r="Q106">
+        <f t="shared" si="10"/>
+        <v>9.1499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q107">
+        <f t="shared" si="10"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s">
+        <v>183</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
         <v>0.06</v>
       </c>
-      <c r="M106">
+      <c r="M108">
         <v>300</v>
       </c>
-      <c r="N106" s="1">
-        <f>C106-D106*20-E106*0.8-F106*0.6-H106*5+I106*10+J106/300</f>
-        <v>-1.2</v>
-      </c>
-      <c r="Q106">
-        <f>P106*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>189</v>
-      </c>
-      <c r="B107" t="s">
-        <v>190</v>
-      </c>
-      <c r="C107">
-        <v>-3</v>
-      </c>
-      <c r="D107">
-        <v>0.19</v>
-      </c>
-      <c r="F107">
-        <v>-1</v>
-      </c>
-      <c r="M107">
-        <v>1200</v>
-      </c>
-      <c r="N107" s="1">
-        <f>C107-D107*20-E107*0.8-F107*0.6-H107*5+I107*10+J107/300</f>
-        <v>-6.2</v>
-      </c>
-      <c r="P107">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="Q107">
-        <f>P107*0.013+0.02</f>
-        <v>0.24879999999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N108" s="1">
         <f>C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
-        <v>0</v>
+        <v>-1.2</v>
       </c>
       <c r="Q108">
         <f>P108*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D109">
-        <v>0.06</v>
+        <v>0.19</v>
+      </c>
+      <c r="F109">
+        <v>-1</v>
       </c>
       <c r="M109">
-        <v>300</v>
+        <v>1200</v>
       </c>
       <c r="N109" s="1">
         <f>C109-D109*20-E109*0.8-F109*0.6-H109*5+I109*10+J109/300</f>
-        <v>-1.2</v>
+        <v>-6.2</v>
+      </c>
+      <c r="P109">
+        <v>17.600000000000001</v>
       </c>
       <c r="Q109">
         <f>P109*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>193</v>
-      </c>
-      <c r="B110" t="s">
-        <v>194</v>
-      </c>
-      <c r="C110">
-        <v>-3</v>
-      </c>
-      <c r="D110">
-        <v>0.25</v>
-      </c>
-      <c r="F110">
-        <v>-2</v>
-      </c>
-      <c r="M110">
-        <v>950</v>
-      </c>
+        <v>0.24879999999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N110" s="1">
         <f>C110-D110*20-E110*0.8-F110*0.6-H110*5+I110*10+J110/300</f>
-        <v>-6.8</v>
-      </c>
-      <c r="P110">
-        <v>17.460599999999999</v>
+        <v>0</v>
       </c>
       <c r="Q110">
         <f>P110*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>186</v>
+      </c>
+      <c r="B111" t="s">
+        <v>187</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0.06</v>
+      </c>
+      <c r="M111">
+        <v>300</v>
+      </c>
+      <c r="N111" s="1">
+        <f>C111-D111*20-E111*0.8-F111*0.6-H111*5+I111*10+J111/300</f>
+        <v>-1.2</v>
+      </c>
+      <c r="Q111">
+        <f>P111*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112">
+        <v>-3</v>
+      </c>
+      <c r="D112">
+        <v>0.25</v>
+      </c>
+      <c r="F112">
+        <v>-2</v>
+      </c>
+      <c r="M112">
+        <v>950</v>
+      </c>
+      <c r="N112" s="1">
+        <f>C112-D112*20-E112*0.8-F112*0.6-H112*5+I112*10+J112/300</f>
+        <v>-6.8</v>
+      </c>
+      <c r="P112">
+        <v>17.460599999999999</v>
+      </c>
+      <c r="Q112">
+        <f>P112*0.013+0.02</f>
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N111" s="1">
-        <f t="shared" ref="N111:N148" si="12">C111-D111*20-E111*0.8-F111*0.6-H111*5+I111*10+J111/300</f>
-        <v>0</v>
-      </c>
-      <c r="Q111">
-        <f t="shared" ref="Q111:Q165" si="13">P111*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>195</v>
-      </c>
-      <c r="B112" t="s">
-        <v>196</v>
-      </c>
-      <c r="C112">
-        <v>0</v>
-      </c>
-      <c r="D112">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N113" s="1">
+        <f t="shared" ref="N113:N150" si="12">C113-D113*20-E113*0.8-F113*0.6-H113*5+I113*10+J113/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q113">
+        <f t="shared" ref="Q113:Q167" si="13">P113*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
         <v>0.06</v>
       </c>
-      <c r="M112">
+      <c r="M114">
         <v>400</v>
       </c>
-      <c r="N112" s="1">
+      <c r="N114" s="1">
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
-      <c r="Q112">
+      <c r="Q114">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>197</v>
-      </c>
-      <c r="B113" t="s">
-        <v>198</v>
-      </c>
-      <c r="C113">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" t="s">
+        <v>193</v>
+      </c>
+      <c r="C115">
         <v>-3</v>
       </c>
-      <c r="D113">
+      <c r="D115">
         <v>0.16</v>
       </c>
-      <c r="M113">
+      <c r="M115">
         <v>750</v>
       </c>
-      <c r="N113" s="1">
+      <c r="N115" s="1">
         <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
-      <c r="P113">
+      <c r="P115">
         <v>10.5822</v>
       </c>
-      <c r="Q113">
+      <c r="Q115">
         <f t="shared" si="13"/>
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N114" s="1">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N116" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q114">
+      <c r="Q116">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>199</v>
-      </c>
-      <c r="B115" t="s">
-        <v>200</v>
-      </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-      <c r="D115">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>194</v>
+      </c>
+      <c r="B117" t="s">
+        <v>195</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
         <v>0.06</v>
       </c>
-      <c r="M115">
+      <c r="M117">
         <v>400</v>
       </c>
-      <c r="N115" s="1">
+      <c r="N117" s="1">
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
-      <c r="Q115">
+      <c r="Q117">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>201</v>
-      </c>
-      <c r="B116" t="s">
-        <v>202</v>
-      </c>
-      <c r="C116">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>196</v>
+      </c>
+      <c r="B118" t="s">
+        <v>197</v>
+      </c>
+      <c r="C118">
         <v>-3.5</v>
       </c>
-      <c r="D116">
+      <c r="D118">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M116">
+      <c r="M118">
         <v>750</v>
       </c>
-      <c r="N116" s="1">
+      <c r="N118" s="1">
         <f t="shared" si="12"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P116">
+      <c r="P118">
         <v>9.5239700000000003</v>
       </c>
-      <c r="Q116">
+      <c r="Q118">
         <f t="shared" si="13"/>
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>203</v>
-      </c>
-      <c r="B117" t="s">
-        <v>204</v>
-      </c>
-      <c r="C117">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>198</v>
+      </c>
+      <c r="B119" t="s">
+        <v>199</v>
+      </c>
+      <c r="C119">
         <v>-3</v>
       </c>
-      <c r="D117">
+      <c r="D119">
         <v>0.16</v>
       </c>
-      <c r="M117">
+      <c r="M119">
         <v>800</v>
       </c>
-      <c r="N117" s="1">
+      <c r="N119" s="1">
         <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
-      <c r="Q117">
+      <c r="Q119">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N118" s="1">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N120" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q118">
+      <c r="Q120">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>207</v>
-      </c>
-      <c r="B119" t="s">
-        <v>208</v>
-      </c>
-      <c r="C119">
-        <v>0</v>
-      </c>
-      <c r="D119">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>202</v>
+      </c>
+      <c r="B121" t="s">
+        <v>203</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
         <v>0.06</v>
       </c>
-      <c r="M119">
+      <c r="M121">
         <v>400</v>
       </c>
-      <c r="N119" s="1">
+      <c r="N121" s="1">
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
-      <c r="P119">
+      <c r="P121">
         <v>4</v>
       </c>
-      <c r="Q119">
+      <c r="Q121">
         <f t="shared" si="13"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S119" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>205</v>
-      </c>
-      <c r="B120" t="s">
-        <v>206</v>
-      </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-      <c r="D120">
+      <c r="S121" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>200</v>
+      </c>
+      <c r="B122" t="s">
+        <v>201</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
         <v>0.06</v>
       </c>
-      <c r="M120">
+      <c r="M122">
         <v>400</v>
       </c>
-      <c r="N120" s="1">
+      <c r="N122" s="1">
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
-      <c r="Q120">
+      <c r="Q122">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>209</v>
-      </c>
-      <c r="B121" t="s">
-        <v>210</v>
-      </c>
-      <c r="C121">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>204</v>
+      </c>
+      <c r="B123" t="s">
+        <v>205</v>
+      </c>
+      <c r="C123">
         <v>-3</v>
       </c>
-      <c r="D121">
+      <c r="D123">
         <v>0.18</v>
       </c>
-      <c r="F121">
+      <c r="F123">
         <v>-1</v>
       </c>
-      <c r="M121">
+      <c r="M123">
         <v>1000</v>
       </c>
-      <c r="N121" s="1">
+      <c r="N123" s="1">
         <f t="shared" si="12"/>
         <v>-6</v>
       </c>
-      <c r="P121">
+      <c r="P123">
         <v>16.600000000000001</v>
       </c>
-      <c r="Q121">
+      <c r="Q123">
         <f t="shared" si="13"/>
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>257</v>
-      </c>
-      <c r="B122" t="s">
-        <v>210</v>
-      </c>
-      <c r="C122">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>252</v>
+      </c>
+      <c r="B124" t="s">
+        <v>205</v>
+      </c>
+      <c r="C124">
         <v>-3</v>
       </c>
-      <c r="D122">
+      <c r="D124">
         <v>0.18</v>
       </c>
-      <c r="F122">
+      <c r="F124">
         <v>-1</v>
       </c>
-      <c r="M122">
+      <c r="M124">
         <v>1000</v>
       </c>
-      <c r="N122" s="1">
+      <c r="N124" s="1">
         <f t="shared" si="12"/>
         <v>-6</v>
       </c>
-      <c r="Q122">
+      <c r="Q124">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>211</v>
-      </c>
-      <c r="B123" t="s">
-        <v>212</v>
-      </c>
-      <c r="C123">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>206</v>
+      </c>
+      <c r="B125" t="s">
+        <v>207</v>
+      </c>
+      <c r="C125">
         <v>-3</v>
       </c>
-      <c r="D123">
+      <c r="D125">
         <v>0.2</v>
       </c>
-      <c r="F123">
+      <c r="F125">
         <v>-2</v>
       </c>
-      <c r="M123">
+      <c r="M125">
         <v>1900</v>
       </c>
-      <c r="N123" s="1">
+      <c r="N125" s="1">
         <f t="shared" si="12"/>
         <v>-5.8</v>
       </c>
-      <c r="P123">
+      <c r="P125">
         <v>14</v>
       </c>
-      <c r="Q123">
+      <c r="Q125">
         <f t="shared" si="13"/>
         <v>0.20199999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>258</v>
-      </c>
-      <c r="B124" t="s">
-        <v>212</v>
-      </c>
-      <c r="C124">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>253</v>
+      </c>
+      <c r="B126" t="s">
+        <v>207</v>
+      </c>
+      <c r="C126">
         <v>-3</v>
       </c>
-      <c r="D124">
+      <c r="D126">
         <v>0.2</v>
       </c>
-      <c r="F124">
+      <c r="F126">
         <v>-2</v>
       </c>
-      <c r="M124">
+      <c r="M126">
         <v>1900</v>
       </c>
-      <c r="N124" s="1">
+      <c r="N126" s="1">
         <f t="shared" si="12"/>
         <v>-5.8</v>
       </c>
-      <c r="Q124">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>261</v>
-      </c>
-      <c r="B125" t="s">
-        <v>262</v>
-      </c>
-      <c r="C125">
-        <v>-3</v>
-      </c>
-      <c r="D125">
-        <v>0.16</v>
-      </c>
-      <c r="F125">
-        <v>-1</v>
-      </c>
-      <c r="M125">
-        <v>1500</v>
-      </c>
-      <c r="N125" s="1">
-        <f t="shared" si="12"/>
-        <v>-5.6000000000000005</v>
-      </c>
-      <c r="P125">
-        <v>10.9</v>
-      </c>
-      <c r="Q125">
-        <f t="shared" si="13"/>
-        <v>0.16169999999999998</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>263</v>
-      </c>
-      <c r="B126" t="s">
-        <v>262</v>
-      </c>
-      <c r="C126">
-        <v>-3</v>
-      </c>
-      <c r="D126">
-        <v>0.16</v>
-      </c>
-      <c r="F126">
-        <v>-1</v>
-      </c>
-      <c r="M126">
-        <v>1500</v>
-      </c>
-      <c r="N126" s="1">
-        <f t="shared" si="12"/>
-        <v>-5.6000000000000005</v>
-      </c>
       <c r="Q126">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B127" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C127">
         <v>-3</v>
@@ -5118,26 +5113,26 @@
         <v>-1</v>
       </c>
       <c r="M127">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="N127" s="1">
         <f t="shared" si="12"/>
         <v>-5.6000000000000005</v>
       </c>
       <c r="P127">
-        <v>10.5</v>
+        <v>10.9</v>
       </c>
       <c r="Q127">
         <f t="shared" si="13"/>
-        <v>0.15649999999999997</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0.16169999999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B128" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C128">
         <v>-3</v>
@@ -5149,7 +5144,7 @@
         <v>-1</v>
       </c>
       <c r="M128">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="N128" s="1">
         <f t="shared" si="12"/>
@@ -5160,12 +5155,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B129" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C129">
         <v>-3</v>
@@ -5177,23 +5172,26 @@
         <v>-1</v>
       </c>
       <c r="M129">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N129" s="1">
         <f t="shared" si="12"/>
         <v>-5.6000000000000005</v>
       </c>
+      <c r="P129">
+        <v>10.5</v>
+      </c>
       <c r="Q129">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.15649999999999997</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B130" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C130">
         <v>-3</v>
@@ -5205,7 +5203,7 @@
         <v>-1</v>
       </c>
       <c r="M130">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N130" s="1">
         <f t="shared" si="12"/>
@@ -5216,216 +5214,222 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>261</v>
+      </c>
+      <c r="B131" t="s">
+        <v>264</v>
+      </c>
+      <c r="C131">
+        <v>-3</v>
+      </c>
+      <c r="D131">
+        <v>0.16</v>
+      </c>
+      <c r="F131">
+        <v>-1</v>
+      </c>
+      <c r="M131">
+        <v>1600</v>
+      </c>
       <c r="N131" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="Q131">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B132" t="s">
-        <v>271</v>
+        <v>264</v>
+      </c>
+      <c r="C132">
+        <v>-3</v>
       </c>
       <c r="D132">
-        <v>0.04</v>
+        <v>0.16</v>
+      </c>
+      <c r="F132">
+        <v>-1</v>
       </c>
       <c r="M132">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="N132" s="1">
         <f t="shared" si="12"/>
-        <v>-0.8</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="Q132">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>274</v>
-      </c>
-      <c r="B133" t="s">
-        <v>272</v>
-      </c>
-      <c r="C133">
-        <v>-3</v>
-      </c>
-      <c r="D133">
-        <v>0.2</v>
-      </c>
-      <c r="F133">
-        <v>-1</v>
-      </c>
-      <c r="M133">
-        <v>1000</v>
-      </c>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N133" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
-      </c>
-      <c r="P133">
-        <v>16.54</v>
+        <v>0</v>
       </c>
       <c r="Q133">
         <f t="shared" si="13"/>
-        <v>0.23501999999999998</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B134" t="s">
-        <v>273</v>
-      </c>
-      <c r="C134">
-        <v>-3</v>
+        <v>266</v>
       </c>
       <c r="D134">
-        <v>0.2</v>
-      </c>
-      <c r="F134">
-        <v>-1</v>
+        <v>0.04</v>
       </c>
       <c r="M134">
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="N134" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
+        <v>-0.8</v>
       </c>
       <c r="Q134">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>269</v>
+      </c>
+      <c r="B135" t="s">
+        <v>267</v>
+      </c>
+      <c r="C135">
+        <v>-3</v>
+      </c>
+      <c r="D135">
+        <v>0.2</v>
+      </c>
+      <c r="F135">
+        <v>-1</v>
+      </c>
+      <c r="M135">
+        <v>1000</v>
+      </c>
       <c r="N135" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-6.4</v>
+      </c>
+      <c r="P135">
+        <v>16.54</v>
       </c>
       <c r="Q135">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.23501999999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>213</v>
+        <v>270</v>
       </c>
       <c r="B136" t="s">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="C136">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="D136">
-        <v>0.06</v>
+        <v>0.2</v>
+      </c>
+      <c r="F136">
+        <v>-1</v>
       </c>
       <c r="M136">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="N136" s="1">
         <f t="shared" si="12"/>
-        <v>-1.7</v>
-      </c>
-      <c r="P136">
-        <v>6.5</v>
+        <v>-6.4</v>
       </c>
       <c r="Q136">
         <f t="shared" si="13"/>
-        <v>0.1045</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>231</v>
-      </c>
-      <c r="B137" t="s">
-        <v>232</v>
-      </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-      <c r="D137">
-        <v>0.01</v>
-      </c>
-      <c r="M137">
-        <v>0</v>
-      </c>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N137" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="Q137">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="B138" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D138">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="M138">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="N138" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-1.7</v>
+      </c>
+      <c r="P138">
+        <v>6.5</v>
       </c>
       <c r="Q138">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1045</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B139" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="C139">
         <v>0</v>
       </c>
       <c r="D139">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M139">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N139" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="Q139">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B140" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -5445,864 +5449,914 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B141" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C141">
         <v>0</v>
       </c>
       <c r="D141">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M141">
         <v>200</v>
       </c>
       <c r="N141" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-0.4</v>
       </c>
       <c r="Q141">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B142" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C142">
         <v>0</v>
       </c>
       <c r="D142">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M142">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N142" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="Q142">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B143" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C143">
         <v>0</v>
       </c>
       <c r="D143">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M143">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N143" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="Q143">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="B144" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C144">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="M144">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="N144" s="1">
         <f t="shared" si="12"/>
-        <v>-3.2</v>
-      </c>
-      <c r="P144">
-        <v>8.6999999999999993</v>
+        <v>-0.4</v>
       </c>
       <c r="Q144">
         <f t="shared" si="13"/>
-        <v>0.1331</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B145" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="C145">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M145">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="N145" s="1">
         <f t="shared" si="12"/>
-        <v>-3.5</v>
-      </c>
-      <c r="P145">
-        <v>7.5</v>
+        <v>-0.4</v>
       </c>
       <c r="Q145">
         <f t="shared" si="13"/>
-        <v>0.11749999999999999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B146" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C146">
         <v>-1</v>
       </c>
       <c r="D146">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="M146">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="N146" s="1">
         <f t="shared" si="12"/>
-        <v>-2.8</v>
+        <v>-3.2</v>
       </c>
       <c r="P146">
-        <v>6.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q146">
         <f t="shared" si="13"/>
-        <v>0.1071</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1331</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B147" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C147">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="D147">
         <v>0.1</v>
       </c>
       <c r="M147">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="N147" s="1">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-3.5</v>
+      </c>
+      <c r="P147">
+        <v>7.5</v>
       </c>
       <c r="Q147">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.11749999999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B148" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C148">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="D148">
-        <v>0.27</v>
-      </c>
-      <c r="F148">
-        <v>-2</v>
+        <v>0.09</v>
       </c>
       <c r="M148">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="N148" s="1">
         <f t="shared" si="12"/>
-        <v>-9.2000000000000011</v>
+        <v>-2.8</v>
       </c>
       <c r="P148">
-        <v>20.100000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="Q148">
         <f t="shared" si="13"/>
-        <v>0.28130000000000005</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>216</v>
+      </c>
+      <c r="B149" t="s">
+        <v>217</v>
+      </c>
+      <c r="C149">
+        <v>-1</v>
+      </c>
+      <c r="D149">
+        <v>0.1</v>
+      </c>
+      <c r="M149">
+        <v>500</v>
+      </c>
       <c r="N149" s="1">
-        <f t="shared" ref="N149:N166" si="14">C149-D149*20-E149*0.8-F149*0.6-H149*5+I149*10+J149/300</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-3</v>
       </c>
       <c r="Q149">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B150" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C150">
+        <v>-5</v>
+      </c>
+      <c r="D150">
+        <v>0.27</v>
+      </c>
+      <c r="F150">
+        <v>-2</v>
+      </c>
+      <c r="M150">
+        <v>4000</v>
+      </c>
+      <c r="N150" s="1">
+        <f t="shared" si="12"/>
+        <v>-9.2000000000000011</v>
+      </c>
+      <c r="P150">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q150">
+        <f t="shared" si="13"/>
+        <v>0.28130000000000005</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N151" s="1">
+        <f t="shared" ref="N151:N168" si="14">C151-D151*20-E151*0.8-F151*0.6-H151*5+I151*10+J151/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q151">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>222</v>
+      </c>
+      <c r="B152" t="s">
+        <v>223</v>
+      </c>
+      <c r="C152">
         <v>-0.5</v>
       </c>
-      <c r="D150">
+      <c r="D152">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M150">
+      <c r="M152">
         <v>1000</v>
       </c>
-      <c r="N150" s="1">
+      <c r="N152" s="1">
         <f t="shared" si="14"/>
         <v>-1.9000000000000001</v>
       </c>
-      <c r="P150">
+      <c r="P152">
         <v>6.6</v>
       </c>
-      <c r="Q150">
+      <c r="Q152">
         <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>233</v>
-      </c>
-      <c r="B151" t="s">
-        <v>234</v>
-      </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-      <c r="D151">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>228</v>
+      </c>
+      <c r="B153" t="s">
+        <v>229</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
         <v>0.01</v>
       </c>
-      <c r="M151">
-        <v>0</v>
-      </c>
-      <c r="N151" s="1">
+      <c r="M153">
+        <v>0</v>
+      </c>
+      <c r="N153" s="1">
         <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
-      <c r="Q151">
-        <f>P151*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>235</v>
-      </c>
-      <c r="B152" t="s">
-        <v>236</v>
-      </c>
-      <c r="C152">
-        <v>0</v>
-      </c>
-      <c r="D152">
+      <c r="Q153">
+        <f>P153*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>230</v>
+      </c>
+      <c r="B154" t="s">
+        <v>231</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
         <v>0.03</v>
       </c>
-      <c r="M152">
+      <c r="M154">
         <v>200</v>
       </c>
-      <c r="N152" s="1">
+      <c r="N154" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q152">
-        <f>P152*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>239</v>
-      </c>
-      <c r="B153" t="s">
-        <v>236</v>
-      </c>
-      <c r="C153">
-        <v>0</v>
-      </c>
-      <c r="D153">
+      <c r="Q154">
+        <f>P154*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>234</v>
+      </c>
+      <c r="B155" t="s">
+        <v>231</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
         <v>0.03</v>
       </c>
-      <c r="M153">
+      <c r="M155">
         <v>200</v>
       </c>
-      <c r="N153" s="1">
+      <c r="N155" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q153">
-        <f>P153*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>229</v>
-      </c>
-      <c r="B154" t="s">
-        <v>230</v>
-      </c>
-      <c r="C154">
+      <c r="Q155">
+        <f>P155*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>224</v>
+      </c>
+      <c r="B156" t="s">
+        <v>225</v>
+      </c>
+      <c r="C156">
         <v>-1</v>
       </c>
-      <c r="D154">
+      <c r="D156">
         <v>0.11</v>
       </c>
-      <c r="M154">
+      <c r="M156">
         <v>500</v>
       </c>
-      <c r="N154" s="1">
+      <c r="N156" s="1">
         <f t="shared" si="14"/>
         <v>-3.2</v>
       </c>
-      <c r="P154">
+      <c r="P156">
         <v>7.0195183999999999</v>
       </c>
-      <c r="Q154">
+      <c r="Q156">
         <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>225</v>
-      </c>
-      <c r="B155" t="s">
-        <v>226</v>
-      </c>
-      <c r="C155">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>220</v>
+      </c>
+      <c r="B157" t="s">
+        <v>221</v>
+      </c>
+      <c r="C157">
         <v>-7</v>
       </c>
-      <c r="D155">
+      <c r="D157">
         <v>0.42</v>
       </c>
-      <c r="F155">
+      <c r="F157">
         <v>-4</v>
       </c>
-      <c r="M155">
+      <c r="M157">
         <v>5000</v>
       </c>
-      <c r="N155" s="1">
+      <c r="N157" s="1">
         <f t="shared" si="14"/>
         <v>-13</v>
       </c>
-      <c r="P155">
+      <c r="P157">
         <v>39.299999999999997</v>
       </c>
-      <c r="Q155">
+      <c r="Q157">
         <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N156" s="1"/>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>278</v>
-      </c>
-      <c r="B157" t="s">
-        <v>279</v>
-      </c>
-      <c r="C157">
-        <v>0</v>
-      </c>
-      <c r="D157">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N158" s="1"/>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>273</v>
+      </c>
+      <c r="B159" t="s">
+        <v>274</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
         <v>0.05</v>
       </c>
-      <c r="M157">
+      <c r="M159">
         <v>400</v>
       </c>
-      <c r="N157" s="1">
+      <c r="N159" s="1">
         <f t="shared" si="14"/>
         <v>-1</v>
       </c>
-      <c r="Q157">
+      <c r="Q159">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B158" s="1" t="s">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C160" s="1">
         <v>-2</v>
       </c>
-      <c r="D158" s="1">
+      <c r="D160" s="1">
         <v>0.16</v>
       </c>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="1"/>
-      <c r="I158" s="1"/>
-      <c r="J158" s="1"/>
-      <c r="K158" s="1"/>
-      <c r="L158" s="1"/>
-      <c r="M158" s="1">
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1">
         <v>1000</v>
       </c>
-      <c r="N158" s="1">
+      <c r="N160" s="1">
         <f t="shared" si="14"/>
         <v>-5.2</v>
       </c>
-      <c r="P158">
+      <c r="P160">
         <v>15</v>
       </c>
-      <c r="Q158">
+      <c r="Q160">
         <f t="shared" si="13"/>
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
-      <c r="H159" s="1"/>
-      <c r="I159" s="1"/>
-      <c r="J159" s="1"/>
-      <c r="K159" s="1"/>
-      <c r="L159" s="1"/>
-      <c r="M159" s="1"/>
-      <c r="N159" s="1"/>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>164</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>165</v>
       </c>
-      <c r="C160">
+      <c r="C162">
         <v>-2.5</v>
       </c>
-      <c r="D160">
+      <c r="D162">
         <v>0.22</v>
       </c>
-      <c r="F160">
+      <c r="F162">
         <v>-1</v>
       </c>
-      <c r="M160">
+      <c r="M162">
         <v>1000</v>
       </c>
-      <c r="N160" s="1">
+      <c r="N162" s="1">
         <f t="shared" si="14"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P160">
+      <c r="P162">
         <v>15.4</v>
       </c>
-      <c r="Q160">
+      <c r="Q162">
         <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
         <v>166</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>167</v>
       </c>
-      <c r="C161">
+      <c r="C163">
         <v>-5</v>
       </c>
-      <c r="D161">
+      <c r="D163">
         <v>0.26</v>
       </c>
-      <c r="F161">
+      <c r="F163">
         <v>-2</v>
       </c>
-      <c r="M161">
+      <c r="M163">
         <v>2000</v>
       </c>
-      <c r="N161" s="1">
+      <c r="N163" s="1">
         <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P161">
+      <c r="P163">
         <v>17.3</v>
       </c>
-      <c r="Q161">
+      <c r="Q163">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>169</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>170</v>
       </c>
-      <c r="C162">
+      <c r="C164">
         <v>-3</v>
       </c>
-      <c r="D162">
+      <c r="D164">
         <v>0.33</v>
       </c>
-      <c r="F162">
+      <c r="F164">
         <v>-3</v>
       </c>
-      <c r="M162">
+      <c r="M164">
         <v>3000</v>
       </c>
-      <c r="N162" s="1">
+      <c r="N164" s="1">
         <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P162">
+      <c r="P164">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q162">
+      <c r="Q164">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>171</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>172</v>
       </c>
-      <c r="C163">
+      <c r="C165">
         <v>-3</v>
       </c>
-      <c r="D163">
+      <c r="D165">
         <v>0.24</v>
       </c>
-      <c r="F163">
+      <c r="F165">
         <v>-2</v>
       </c>
-      <c r="M163">
+      <c r="M165">
         <v>3000</v>
       </c>
-      <c r="N163" s="1">
+      <c r="N165" s="1">
         <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P163">
+      <c r="P165">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q163">
+      <c r="Q165">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>173</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>174</v>
       </c>
-      <c r="C164">
+      <c r="C166">
         <v>-3</v>
       </c>
-      <c r="D164">
+      <c r="D166">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F164">
+      <c r="F166">
         <v>-1</v>
       </c>
-      <c r="M164">
+      <c r="M166">
         <v>4000</v>
       </c>
-      <c r="N164" s="1">
+      <c r="N166" s="1">
         <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P164">
+      <c r="P166">
         <v>21.9</v>
       </c>
-      <c r="Q164">
+      <c r="Q166">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>175</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>176</v>
       </c>
-      <c r="C165">
+      <c r="C167">
         <v>-3</v>
       </c>
-      <c r="D165">
+      <c r="D167">
         <v>0.27</v>
       </c>
-      <c r="F165">
+      <c r="F167">
         <v>-2</v>
       </c>
-      <c r="M165">
+      <c r="M167">
         <v>2000</v>
       </c>
-      <c r="N165" s="1">
+      <c r="N167" s="1">
         <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P165">
+      <c r="P167">
         <v>19.3</v>
       </c>
-      <c r="Q165">
+      <c r="Q167">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N166" s="1">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N168" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q166">
-        <f>P166*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>253</v>
-      </c>
-      <c r="B167" t="s">
-        <v>254</v>
-      </c>
-      <c r="C167">
+      <c r="Q168">
+        <f>P168*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>248</v>
+      </c>
+      <c r="B169" t="s">
+        <v>249</v>
+      </c>
+      <c r="C169">
         <v>-2</v>
       </c>
-      <c r="D167">
+      <c r="D169">
         <v>0.05</v>
       </c>
-      <c r="M167">
+      <c r="M169">
         <v>300</v>
       </c>
-      <c r="N167" s="1"/>
-      <c r="Q167">
-        <f t="shared" ref="Q167:Q178" si="15">P167*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>249</v>
-      </c>
-      <c r="B168" t="s">
+      <c r="N169" s="1"/>
+      <c r="Q169">
+        <f t="shared" ref="Q169:Q180" si="15">P169*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>244</v>
+      </c>
+      <c r="B170" t="s">
+        <v>245</v>
+      </c>
+      <c r="C170">
+        <v>-2</v>
+      </c>
+      <c r="D170">
+        <v>0.05</v>
+      </c>
+      <c r="M170">
+        <v>300</v>
+      </c>
+      <c r="N170" s="1"/>
+      <c r="Q170">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
         <v>250</v>
       </c>
-      <c r="C168">
-        <v>-2</v>
-      </c>
-      <c r="D168">
-        <v>0.05</v>
-      </c>
-      <c r="M168">
-        <v>300</v>
-      </c>
-      <c r="N168" s="1"/>
-      <c r="Q168">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>255</v>
-      </c>
-      <c r="B169" t="s">
-        <v>256</v>
-      </c>
-      <c r="C169">
+      <c r="B171" t="s">
+        <v>251</v>
+      </c>
+      <c r="C171">
         <v>-3</v>
       </c>
-      <c r="D169">
+      <c r="D171">
         <v>0.17</v>
       </c>
-      <c r="M169">
+      <c r="M171">
         <v>750</v>
       </c>
-      <c r="N169" s="1"/>
-      <c r="P169">
+      <c r="N171" s="1"/>
+      <c r="P171">
         <v>13.3</v>
       </c>
-      <c r="Q169">
-        <f>P169*0.013+0.02</f>
+      <c r="Q171">
+        <f>P171*0.013+0.02</f>
         <v>0.19289999999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>251</v>
-      </c>
-      <c r="B170" t="s">
-        <v>252</v>
-      </c>
-      <c r="C170">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>246</v>
+      </c>
+      <c r="B172" t="s">
+        <v>247</v>
+      </c>
+      <c r="C172">
         <v>-3</v>
       </c>
-      <c r="D170">
+      <c r="D172">
         <v>0.18</v>
       </c>
-      <c r="M170">
+      <c r="M172">
         <v>1000</v>
       </c>
-      <c r="N170" s="1"/>
-      <c r="P170">
+      <c r="N172" s="1"/>
+      <c r="P172">
         <v>13.28</v>
       </c>
-      <c r="Q170">
-        <f>P170*0.013+0.02</f>
+      <c r="Q172">
+        <f>P172*0.013+0.02</f>
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N171" s="1"/>
-      <c r="Q171">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>259</v>
-      </c>
-      <c r="B172" t="s">
-        <v>260</v>
-      </c>
-      <c r="C172">
-        <v>-8</v>
-      </c>
-      <c r="D172">
-        <v>0.36</v>
-      </c>
-      <c r="F172">
-        <v>-3</v>
-      </c>
-      <c r="M172">
-        <v>3000</v>
-      </c>
-      <c r="N172" s="1"/>
-      <c r="Q172">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N173" s="1"/>
       <c r="Q173">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="B174" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="D174">
-        <v>0.13</v>
+        <v>0.36</v>
+      </c>
+      <c r="F174">
+        <v>-3</v>
       </c>
       <c r="M174">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="N174" s="1"/>
-      <c r="P174">
-        <v>12.1</v>
-      </c>
       <c r="Q174">
         <f t="shared" si="15"/>
-        <v>0.17729999999999999</v>
-      </c>
-    </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>282</v>
-      </c>
-      <c r="B175" t="s">
-        <v>283</v>
-      </c>
-      <c r="C175">
-        <v>-3</v>
-      </c>
-      <c r="D175">
-        <v>0.06</v>
-      </c>
-      <c r="M175">
-        <v>700</v>
-      </c>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N175" s="1"/>
       <c r="Q175">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>275</v>
+      </c>
+      <c r="B176" t="s">
+        <v>276</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>0.13</v>
+      </c>
+      <c r="M176">
+        <v>1000</v>
+      </c>
       <c r="N176" s="1"/>
+      <c r="P176">
+        <v>12.1</v>
+      </c>
       <c r="Q176">
         <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="177" spans="17:17" x14ac:dyDescent="0.25">
+        <v>0.17729999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>277</v>
+      </c>
+      <c r="B177" t="s">
+        <v>278</v>
+      </c>
+      <c r="C177">
+        <v>-3</v>
+      </c>
+      <c r="D177">
+        <v>0.06</v>
+      </c>
+      <c r="M177">
+        <v>700</v>
+      </c>
+      <c r="N177" s="1"/>
       <c r="Q177">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="178" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N178" s="1"/>
       <c r="Q178">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q179">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q180">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>

<commit_message>
oopsie, add back npz optic
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69123B92-5B52-4D1B-A5BD-1F7B008D4D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FB49B3-FCB2-4DA9-9A55-C56F4916270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6255" yWindow="4995" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="317">
   <si>
     <t>new</t>
   </si>
@@ -966,6 +966,24 @@
   </si>
   <si>
     <t>Aimpoint CompM2</t>
+  </si>
+  <si>
+    <t>npz_pso_1_4x24_picatinny_scope</t>
+  </si>
+  <si>
+    <t>NPZ PSO-1 4x24 Picatinny Scope</t>
+  </si>
+  <si>
+    <t>npz_pso_rear_cup</t>
+  </si>
+  <si>
+    <t>NPZ PSO Rear Cup</t>
+  </si>
+  <si>
+    <t>npz_pso_front_cup</t>
+  </si>
+  <si>
+    <t>NPZ PSO Front Cup</t>
   </si>
 </sst>
 </file>
@@ -1807,20 +1825,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S180"/>
+  <dimension ref="A1:S181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J183" sqref="J183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="21" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" customWidth="1"/>
+    <col min="3" max="21" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1838,7 +1856,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1942,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1957,7 +1975,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1990,7 +2008,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2029,7 +2047,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2068,7 +2086,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2107,7 +2125,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +2164,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>298</v>
       </c>
@@ -2182,7 +2200,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2205,7 +2223,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -2238,7 +2256,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -2271,7 +2289,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2304,7 +2322,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2329,7 +2347,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2401,7 +2419,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2424,7 +2442,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2449,7 +2467,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2474,7 +2492,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2499,7 +2517,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N22" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2509,7 +2527,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>300</v>
       </c>
@@ -2534,7 +2552,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2559,7 +2577,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -2584,7 +2602,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -2609,7 +2627,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2634,7 +2652,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2659,7 +2677,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2684,7 +2702,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2709,7 +2727,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2737,7 +2755,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2762,7 +2780,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2787,7 +2805,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2812,7 +2830,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2837,7 +2855,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2862,7 +2880,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2890,7 +2908,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2918,7 +2936,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2943,7 +2961,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2974,7 +2992,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>279</v>
       </c>
@@ -2995,7 +3013,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3026,7 +3044,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -3054,7 +3072,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -3079,7 +3097,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>107</v>
       </c>
@@ -3104,7 +3122,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3129,7 +3147,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3154,7 +3172,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N48" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3164,7 +3182,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -3189,7 +3207,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -3214,7 +3232,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>115</v>
       </c>
@@ -3239,7 +3257,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -3270,7 +3288,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N53" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3280,7 +3298,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -3311,7 +3329,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>120</v>
       </c>
@@ -3342,7 +3360,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>121</v>
       </c>
@@ -3370,7 +3388,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -3401,7 +3419,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -3426,7 +3444,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -3451,7 +3469,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -3476,7 +3494,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -3501,7 +3519,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -3526,7 +3544,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -3554,7 +3572,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -3579,7 +3597,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -3604,7 +3622,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -3629,7 +3647,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -3654,7 +3672,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -3679,7 +3697,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3704,7 +3722,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N70" s="1">
         <f t="shared" ref="N70:N101" si="7">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
         <v>0</v>
@@ -3714,7 +3732,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3739,7 +3757,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>161</v>
       </c>
@@ -3767,7 +3785,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -3792,7 +3810,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N74" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3802,7 +3820,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>302</v>
       </c>
@@ -3827,7 +3845,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>303</v>
       </c>
@@ -3852,7 +3870,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>305</v>
       </c>
@@ -3880,7 +3898,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>307</v>
       </c>
@@ -3901,7 +3919,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>309</v>
       </c>
@@ -3922,7 +3940,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N80" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3932,7 +3950,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -3957,7 +3975,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -3985,7 +4003,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N83" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3995,7 +4013,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>135</v>
       </c>
@@ -4023,7 +4041,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>137</v>
       </c>
@@ -4051,7 +4069,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>139</v>
       </c>
@@ -4079,7 +4097,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -4107,7 +4125,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -4138,7 +4156,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -4169,7 +4187,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>157</v>
       </c>
@@ -4197,7 +4215,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>141</v>
       </c>
@@ -4225,7 +4243,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>149</v>
       </c>
@@ -4253,7 +4271,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>151</v>
       </c>
@@ -4281,7 +4299,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -4306,7 +4324,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>155</v>
       </c>
@@ -4334,7 +4352,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N96" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4344,7 +4362,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>32</v>
       </c>
@@ -4377,7 +4395,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>34</v>
       </c>
@@ -4410,7 +4428,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>53</v>
       </c>
@@ -4435,7 +4453,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>55</v>
       </c>
@@ -4460,7 +4478,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4485,7 +4503,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>57</v>
       </c>
@@ -4513,7 +4531,7 @@
         <v>9.9299999999999999E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>59</v>
       </c>
@@ -4538,7 +4556,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>60</v>
       </c>
@@ -4563,7 +4581,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>61</v>
       </c>
@@ -4588,7 +4606,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -4616,7 +4634,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4639,7 +4657,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>182</v>
       </c>
@@ -4664,7 +4682,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>184</v>
       </c>
@@ -4695,7 +4713,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N110" s="1">
         <f>C110-D110*20-E110*0.8-F110*0.6-H110*5+I110*10+J110/300</f>
         <v>0</v>
@@ -4705,7 +4723,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>186</v>
       </c>
@@ -4730,7 +4748,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>188</v>
       </c>
@@ -4761,7 +4779,7 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N113" s="1">
         <f t="shared" ref="N113:N150" si="12">C113-D113*20-E113*0.8-F113*0.6-H113*5+I113*10+J113/300</f>
         <v>0</v>
@@ -4771,7 +4789,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>190</v>
       </c>
@@ -4796,7 +4814,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>192</v>
       </c>
@@ -4824,7 +4842,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N116" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4834,7 +4852,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>194</v>
       </c>
@@ -4859,7 +4877,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>196</v>
       </c>
@@ -4887,7 +4905,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>198</v>
       </c>
@@ -4912,7 +4930,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N120" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4922,7 +4940,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>202</v>
       </c>
@@ -4953,7 +4971,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -4978,7 +4996,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>204</v>
       </c>
@@ -5009,7 +5027,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -5037,7 +5055,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>206</v>
       </c>
@@ -5068,7 +5086,7 @@
         <v>0.20199999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>253</v>
       </c>
@@ -5096,7 +5114,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>256</v>
       </c>
@@ -5127,7 +5145,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>258</v>
       </c>
@@ -5155,7 +5173,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>259</v>
       </c>
@@ -5186,7 +5204,7 @@
         <v>0.15649999999999997</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>260</v>
       </c>
@@ -5214,7 +5232,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>261</v>
       </c>
@@ -5242,7 +5260,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -5270,7 +5288,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N133" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5280,7 +5298,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>265</v>
       </c>
@@ -5302,7 +5320,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>269</v>
       </c>
@@ -5333,7 +5351,7 @@
         <v>0.23501999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -5361,7 +5379,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N137" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5371,7 +5389,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -5399,7 +5417,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>226</v>
       </c>
@@ -5424,7 +5442,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>232</v>
       </c>
@@ -5449,7 +5467,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>236</v>
       </c>
@@ -5474,7 +5492,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>235</v>
       </c>
@@ -5499,7 +5517,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>238</v>
       </c>
@@ -5524,7 +5542,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>240</v>
       </c>
@@ -5549,7 +5567,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>242</v>
       </c>
@@ -5574,7 +5592,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>210</v>
       </c>
@@ -5602,7 +5620,7 @@
         <v>0.1331</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>212</v>
       </c>
@@ -5630,7 +5648,7 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>214</v>
       </c>
@@ -5658,7 +5676,7 @@
         <v>0.1071</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>216</v>
       </c>
@@ -5683,7 +5701,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>218</v>
       </c>
@@ -5714,7 +5732,7 @@
         <v>0.28130000000000005</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N151" s="1">
         <f t="shared" ref="N151:N168" si="14">C151-D151*20-E151*0.8-F151*0.6-H151*5+I151*10+J151/300</f>
         <v>0</v>
@@ -5724,7 +5742,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>222</v>
       </c>
@@ -5752,7 +5770,7 @@
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>228</v>
       </c>
@@ -5777,7 +5795,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>230</v>
       </c>
@@ -5802,7 +5820,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>234</v>
       </c>
@@ -5827,7 +5845,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>224</v>
       </c>
@@ -5855,7 +5873,7 @@
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>220</v>
       </c>
@@ -5886,10 +5904,10 @@
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N158" s="1"/>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>273</v>
       </c>
@@ -5914,7 +5932,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>272</v>
       </c>
@@ -5950,7 +5968,7 @@
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5966,7 +5984,7 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>164</v>
       </c>
@@ -5997,7 +6015,7 @@
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -6028,7 +6046,7 @@
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>169</v>
       </c>
@@ -6059,7 +6077,7 @@
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -6090,7 +6108,7 @@
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -6121,7 +6139,7 @@
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>175</v>
       </c>
@@ -6152,7 +6170,7 @@
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N168" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -6162,7 +6180,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>248</v>
       </c>
@@ -6180,11 +6198,11 @@
       </c>
       <c r="N169" s="1"/>
       <c r="Q169">
-        <f t="shared" ref="Q169:Q180" si="15">P169*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Q169:Q181" si="15">P169*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>244</v>
       </c>
@@ -6206,7 +6224,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>250</v>
       </c>
@@ -6231,7 +6249,7 @@
         <v>0.19289999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>246</v>
       </c>
@@ -6256,14 +6274,14 @@
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N173" s="1"/>
       <c r="Q173">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>254</v>
       </c>
@@ -6288,14 +6306,14 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N175" s="1"/>
       <c r="Q175">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>275</v>
       </c>
@@ -6320,7 +6338,7 @@
         <v>0.17729999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>277</v>
       </c>
@@ -6342,21 +6360,75 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N178" s="1"/>
       <c r="Q178">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>311</v>
+      </c>
+      <c r="B179" t="s">
+        <v>312</v>
+      </c>
+      <c r="C179">
+        <v>-3</v>
+      </c>
+      <c r="D179">
+        <v>0.21</v>
+      </c>
+      <c r="F179">
+        <v>-1</v>
+      </c>
+      <c r="M179">
+        <v>1200</v>
+      </c>
       <c r="Q179">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>313</v>
+      </c>
+      <c r="B180" t="s">
+        <v>314</v>
+      </c>
+      <c r="C180">
+        <v>2</v>
+      </c>
+      <c r="D180">
+        <v>0.02</v>
+      </c>
+      <c r="M180">
+        <v>0</v>
+      </c>
       <c r="Q180">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>315</v>
+      </c>
+      <c r="B181" t="s">
+        <v>316</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>0.02</v>
+      </c>
+      <c r="M181">
+        <v>0</v>
+      </c>
+      <c r="Q181">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>

<commit_message>
fix qrp2 + compm4
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FB49B3-FCB2-4DA9-9A55-C56F4916270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AB2B4D-FA8C-4EDB-8E10-0082C3464EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="4995" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="323">
   <si>
     <t>new</t>
   </si>
@@ -984,6 +984,24 @@
   </si>
   <si>
     <t>NPZ PSO Front Cup</t>
+  </si>
+  <si>
+    <t>aimpoint_qrp2_modular_base_mount</t>
+  </si>
+  <si>
+    <t>Aimpoint QRP2 Modular Base Mount</t>
+  </si>
+  <si>
+    <t>aimpoint_ar15_spacer</t>
+  </si>
+  <si>
+    <t>Aimpoint AR-15 Spacer</t>
+  </si>
+  <si>
+    <t>aimpoint_compm4_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint CompM4</t>
   </si>
 </sst>
 </file>
@@ -1529,9 +1547,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1569,7 +1587,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1675,7 +1693,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1817,7 +1835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1825,20 +1843,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S181"/>
+  <dimension ref="A1:S185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J183" sqref="J183"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G182" sqref="G182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="21" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="21" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1856,7 +1874,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1909,7 +1927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1942,7 +1960,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1975,7 +1993,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2008,7 +2026,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2047,7 +2065,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2086,7 +2104,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2125,7 +2143,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2164,7 +2182,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>298</v>
       </c>
@@ -2200,7 +2218,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2223,7 +2241,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -2256,7 +2274,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2322,7 +2340,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2347,7 +2365,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2383,7 +2401,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2419,7 +2437,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2442,7 +2460,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2467,7 +2485,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2492,7 +2510,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2517,7 +2535,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N22" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2527,7 +2545,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>300</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2577,7 +2595,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -2602,7 +2620,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -2627,7 +2645,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2652,7 +2670,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2677,7 +2695,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2702,7 +2720,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2727,7 +2745,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -2755,7 +2773,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2780,7 +2798,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2805,7 +2823,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2830,7 +2848,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -2855,7 +2873,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2880,7 +2898,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2908,7 +2926,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2936,7 +2954,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2961,7 +2979,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2992,7 +3010,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>279</v>
       </c>
@@ -3013,7 +3031,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3044,7 +3062,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -3072,7 +3090,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -3097,7 +3115,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>107</v>
       </c>
@@ -3122,7 +3140,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3147,7 +3165,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3172,7 +3190,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N48" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3182,7 +3200,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -3207,7 +3225,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -3232,7 +3250,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>115</v>
       </c>
@@ -3257,7 +3275,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -3288,7 +3306,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N53" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3298,7 +3316,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -3329,7 +3347,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>120</v>
       </c>
@@ -3360,7 +3378,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>121</v>
       </c>
@@ -3388,7 +3406,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>124</v>
       </c>
@@ -3419,7 +3437,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -3444,7 +3462,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -3469,7 +3487,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -3494,7 +3512,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -3519,7 +3537,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -3544,7 +3562,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -3572,7 +3590,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -3597,7 +3615,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -3622,7 +3640,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -3647,7 +3665,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -3672,7 +3690,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -3697,7 +3715,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3722,7 +3740,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N70" s="1">
         <f t="shared" ref="N70:N101" si="7">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
         <v>0</v>
@@ -3732,7 +3750,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3757,7 +3775,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>161</v>
       </c>
@@ -3785,7 +3803,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -3810,7 +3828,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N74" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3820,7 +3838,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>302</v>
       </c>
@@ -3845,7 +3863,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>303</v>
       </c>
@@ -3870,7 +3888,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>305</v>
       </c>
@@ -3898,7 +3916,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>307</v>
       </c>
@@ -3919,7 +3937,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>309</v>
       </c>
@@ -3940,7 +3958,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N80" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3950,7 +3968,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -3975,7 +3993,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -4003,7 +4021,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N83" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4013,7 +4031,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>135</v>
       </c>
@@ -4041,7 +4059,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>137</v>
       </c>
@@ -4069,7 +4087,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>139</v>
       </c>
@@ -4097,7 +4115,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -4125,7 +4143,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -4156,7 +4174,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -4187,7 +4205,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>157</v>
       </c>
@@ -4215,7 +4233,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>141</v>
       </c>
@@ -4243,7 +4261,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>149</v>
       </c>
@@ -4271,7 +4289,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>151</v>
       </c>
@@ -4299,7 +4317,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -4324,7 +4342,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>155</v>
       </c>
@@ -4352,7 +4370,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N96" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4362,7 +4380,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>32</v>
       </c>
@@ -4395,7 +4413,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>34</v>
       </c>
@@ -4428,7 +4446,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>53</v>
       </c>
@@ -4453,7 +4471,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>55</v>
       </c>
@@ -4478,7 +4496,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4503,7 +4521,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>57</v>
       </c>
@@ -4531,7 +4549,7 @@
         <v>9.9299999999999999E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>59</v>
       </c>
@@ -4556,7 +4574,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>60</v>
       </c>
@@ -4581,7 +4599,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>61</v>
       </c>
@@ -4606,7 +4624,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -4634,7 +4652,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4657,7 +4675,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>182</v>
       </c>
@@ -4682,7 +4700,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>184</v>
       </c>
@@ -4713,7 +4731,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N110" s="1">
         <f>C110-D110*20-E110*0.8-F110*0.6-H110*5+I110*10+J110/300</f>
         <v>0</v>
@@ -4723,7 +4741,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>186</v>
       </c>
@@ -4748,7 +4766,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>188</v>
       </c>
@@ -4779,7 +4797,7 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N113" s="1">
         <f t="shared" ref="N113:N150" si="12">C113-D113*20-E113*0.8-F113*0.6-H113*5+I113*10+J113/300</f>
         <v>0</v>
@@ -4789,7 +4807,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>190</v>
       </c>
@@ -4814,7 +4832,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>192</v>
       </c>
@@ -4842,7 +4860,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N116" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4852,7 +4870,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>194</v>
       </c>
@@ -4877,7 +4895,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>196</v>
       </c>
@@ -4905,7 +4923,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>198</v>
       </c>
@@ -4930,7 +4948,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N120" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4940,7 +4958,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>202</v>
       </c>
@@ -4971,7 +4989,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -4996,7 +5014,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>204</v>
       </c>
@@ -5027,7 +5045,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -5055,7 +5073,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>206</v>
       </c>
@@ -5086,7 +5104,7 @@
         <v>0.20199999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>253</v>
       </c>
@@ -5114,7 +5132,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>256</v>
       </c>
@@ -5145,7 +5163,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>258</v>
       </c>
@@ -5173,7 +5191,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>259</v>
       </c>
@@ -5204,7 +5222,7 @@
         <v>0.15649999999999997</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>260</v>
       </c>
@@ -5232,7 +5250,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>261</v>
       </c>
@@ -5260,7 +5278,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -5288,7 +5306,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N133" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5298,7 +5316,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>265</v>
       </c>
@@ -5320,7 +5338,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>269</v>
       </c>
@@ -5351,7 +5369,7 @@
         <v>0.23501999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -5379,7 +5397,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N137" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5389,7 +5407,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -5417,7 +5435,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>226</v>
       </c>
@@ -5442,7 +5460,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>232</v>
       </c>
@@ -5467,7 +5485,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>236</v>
       </c>
@@ -5492,7 +5510,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>235</v>
       </c>
@@ -5517,7 +5535,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>238</v>
       </c>
@@ -5542,7 +5560,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>240</v>
       </c>
@@ -5567,7 +5585,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>242</v>
       </c>
@@ -5592,7 +5610,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>210</v>
       </c>
@@ -5620,7 +5638,7 @@
         <v>0.1331</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>212</v>
       </c>
@@ -5648,7 +5666,7 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>214</v>
       </c>
@@ -5676,7 +5694,7 @@
         <v>0.1071</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>216</v>
       </c>
@@ -5701,7 +5719,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>218</v>
       </c>
@@ -5732,9 +5750,9 @@
         <v>0.28130000000000005</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N151" s="1">
-        <f t="shared" ref="N151:N168" si="14">C151-D151*20-E151*0.8-F151*0.6-H151*5+I151*10+J151/300</f>
+        <f t="shared" ref="N151:N185" si="14">C151-D151*20-E151*0.8-F151*0.6-H151*5+I151*10+J151/300</f>
         <v>0</v>
       </c>
       <c r="Q151">
@@ -5742,7 +5760,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>222</v>
       </c>
@@ -5770,7 +5788,7 @@
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>228</v>
       </c>
@@ -5795,7 +5813,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>230</v>
       </c>
@@ -5820,7 +5838,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>234</v>
       </c>
@@ -5845,7 +5863,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>224</v>
       </c>
@@ -5873,7 +5891,7 @@
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>220</v>
       </c>
@@ -5904,10 +5922,10 @@
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N158" s="1"/>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>273</v>
       </c>
@@ -5932,7 +5950,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>272</v>
       </c>
@@ -5968,7 +5986,7 @@
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5984,7 +6002,7 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>164</v>
       </c>
@@ -6015,7 +6033,7 @@
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>166</v>
       </c>
@@ -6046,7 +6064,7 @@
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>169</v>
       </c>
@@ -6077,7 +6095,7 @@
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -6108,7 +6126,7 @@
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -6139,7 +6157,7 @@
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>175</v>
       </c>
@@ -6170,7 +6188,7 @@
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N168" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -6180,7 +6198,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>248</v>
       </c>
@@ -6196,13 +6214,16 @@
       <c r="M169">
         <v>300</v>
       </c>
-      <c r="N169" s="1"/>
+      <c r="N169" s="1">
+        <f t="shared" si="14"/>
+        <v>-3</v>
+      </c>
       <c r="Q169">
-        <f t="shared" ref="Q169:Q181" si="15">P169*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q169:Q185" si="15">P169*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>244</v>
       </c>
@@ -6218,13 +6239,16 @@
       <c r="M170">
         <v>300</v>
       </c>
-      <c r="N170" s="1"/>
+      <c r="N170" s="1">
+        <f t="shared" si="14"/>
+        <v>-3</v>
+      </c>
       <c r="Q170">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>250</v>
       </c>
@@ -6240,7 +6264,10 @@
       <c r="M171">
         <v>750</v>
       </c>
-      <c r="N171" s="1"/>
+      <c r="N171" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.4</v>
+      </c>
       <c r="P171">
         <v>13.3</v>
       </c>
@@ -6249,7 +6276,7 @@
         <v>0.19289999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>246</v>
       </c>
@@ -6265,7 +6292,10 @@
       <c r="M172">
         <v>1000</v>
       </c>
-      <c r="N172" s="1"/>
+      <c r="N172" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.6</v>
+      </c>
       <c r="P172">
         <v>13.28</v>
       </c>
@@ -6274,14 +6304,17 @@
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N173" s="1"/>
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N173" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="Q173">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>254</v>
       </c>
@@ -6300,20 +6333,26 @@
       <c r="M174">
         <v>3000</v>
       </c>
-      <c r="N174" s="1"/>
+      <c r="N174" s="1">
+        <f t="shared" si="14"/>
+        <v>-13.399999999999999</v>
+      </c>
       <c r="Q174">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N175" s="1"/>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N175" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="Q175">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>275</v>
       </c>
@@ -6329,7 +6368,10 @@
       <c r="M176">
         <v>1000</v>
       </c>
-      <c r="N176" s="1"/>
+      <c r="N176" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.6</v>
+      </c>
       <c r="P176">
         <v>12.1</v>
       </c>
@@ -6338,7 +6380,7 @@
         <v>0.17729999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>277</v>
       </c>
@@ -6354,20 +6396,26 @@
       <c r="M177">
         <v>700</v>
       </c>
-      <c r="N177" s="1"/>
+      <c r="N177" s="1">
+        <f t="shared" si="14"/>
+        <v>-4.2</v>
+      </c>
       <c r="Q177">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N178" s="1"/>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N178" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="Q178">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>311</v>
       </c>
@@ -6386,12 +6434,16 @@
       <c r="M179">
         <v>1200</v>
       </c>
+      <c r="N179" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.6000000000000005</v>
+      </c>
       <c r="Q179">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>313</v>
       </c>
@@ -6407,12 +6459,16 @@
       <c r="M180">
         <v>0</v>
       </c>
+      <c r="N180" s="1">
+        <f t="shared" si="14"/>
+        <v>1.6</v>
+      </c>
       <c r="Q180">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>315</v>
       </c>
@@ -6428,9 +6484,104 @@
       <c r="M181">
         <v>0</v>
       </c>
+      <c r="N181" s="1">
+        <f t="shared" si="14"/>
+        <v>0.6</v>
+      </c>
       <c r="Q181">
         <f t="shared" si="15"/>
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N182" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q182">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>317</v>
+      </c>
+      <c r="B183" t="s">
+        <v>318</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0.03</v>
+      </c>
+      <c r="M183">
+        <v>300</v>
+      </c>
+      <c r="N183" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.6</v>
+      </c>
+      <c r="P183">
+        <v>11.8</v>
+      </c>
+      <c r="Q183">
+        <f t="shared" si="15"/>
+        <v>0.1734</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>319</v>
+      </c>
+      <c r="B184" t="s">
+        <v>320</v>
+      </c>
+      <c r="C184">
+        <v>-1</v>
+      </c>
+      <c r="D184">
+        <v>0.02</v>
+      </c>
+      <c r="M184">
+        <v>200</v>
+      </c>
+      <c r="N184" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.4</v>
+      </c>
+      <c r="Q184">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>321</v>
+      </c>
+      <c r="B185" t="s">
+        <v>322</v>
+      </c>
+      <c r="C185">
+        <v>-1</v>
+      </c>
+      <c r="D185">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M185">
+        <v>1000</v>
+      </c>
+      <c r="N185" s="1">
+        <f t="shared" si="14"/>
+        <v>-3.8000000000000003</v>
+      </c>
+      <c r="P185">
+        <v>9.4</v>
+      </c>
+      <c r="Q185">
+        <f t="shared" si="15"/>
+        <v>0.14219999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>